<commit_message>
Enhance job matching and PDF generation workflows with new scripts for email scraping and classification. Introduced Gmail response tracking scripts, including email data analysis, classification framework, and email scraping functionalities. Updated configuration files and documentation for improved clarity and usability. Adjusted Greenhouse job matching settings for better processing accuracy.
</commit_message>
<xml_diff>
--- a/Phase 2 Workflow/Education_treatment_final.xlsx
+++ b/Phase 2 Workflow/Education_treatment_final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://humberital-my.sharepoint.com/personal/n01609495_humber_ca/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://humberital-my.sharepoint.com/personal/n01780947_humber_ca/Documents/Documents/Repos/resume_parsing_audit_study/Phase 2 Workflow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{44B18F12-6C27-4BD4-89CF-3E5597C3B23A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="14_{44B18F12-6C27-4BD4-89CF-3E5597C3B23A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B026520-49BE-490C-B0EB-6DCF1FF13F9A}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{886D032E-E60D-4ED1-BE85-59C2C553EBD4}"/>
+    <workbookView xWindow="-23148" yWindow="8640" windowWidth="23256" windowHeight="13896" xr2:uid="{886D032E-E60D-4ED1-BE85-59C2C553EBD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Education_treatment_augmented" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="62">
   <si>
     <t>treatment_primary_key</t>
   </si>
@@ -103,12 +103,6 @@
     <t>MSfE</t>
   </si>
   <si>
-    <t>Manufacturing Systems for Engineers Certificate</t>
-  </si>
-  <si>
-    <t>Manufacturing Systems for Engineers Bridging Certificate</t>
-  </si>
-  <si>
     <t>DMC</t>
   </si>
   <si>
@@ -194,13 +188,34 @@
   </si>
   <si>
     <t>Community Health Care Connections Certificate</t>
+  </si>
+  <si>
+    <t>FSCeF</t>
+  </si>
+  <si>
+    <t>Collège Boréal – ACCES Employment</t>
+  </si>
+  <si>
+    <t>Financial Services Connections En Français</t>
+  </si>
+  <si>
+    <t>Collège Boréal (In collaboration with ACCES Employment)</t>
+  </si>
+  <si>
+    <t>Financial Services Connections Certificate (En Français)</t>
+  </si>
+  <si>
+    <t>Microsoft Skills Bridging Program</t>
+  </si>
+  <si>
+    <t>Microsoft  Bridging Program</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,6 +346,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -677,9 +699,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1055,20 +1078,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{441BF3D2-3897-4F5E-B9B0-D6AC4D88AB22}">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="62.15625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.1015625" customWidth="1"/>
-    <col min="5" max="5" width="19.9453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.08984375" customWidth="1"/>
+    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1085,7 +1108,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1102,7 +1125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1119,7 +1142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1136,7 +1159,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1153,7 +1176,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1170,7 +1193,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1187,415 +1210,415 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
         <v>53</v>
       </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s">
-        <v>55</v>
-      </c>
       <c r="E9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E10">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
         <v>53</v>
       </c>
-      <c r="C12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" t="s">
-        <v>55</v>
-      </c>
       <c r="E12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E13">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
         <v>28</v>
       </c>
-      <c r="C14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" t="s">
-        <v>30</v>
-      </c>
       <c r="E14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" t="s">
         <v>29</v>
       </c>
-      <c r="D15" t="s">
-        <v>31</v>
-      </c>
       <c r="E15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
         <v>28</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" t="s">
-        <v>30</v>
       </c>
       <c r="E16">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" t="s">
         <v>28</v>
       </c>
-      <c r="C18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" t="s">
-        <v>30</v>
-      </c>
       <c r="E18">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" t="s">
         <v>28</v>
-      </c>
-      <c r="C19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" t="s">
-        <v>30</v>
       </c>
       <c r="E19">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" t="s">
         <v>49</v>
       </c>
-      <c r="C21" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" t="s">
-        <v>51</v>
-      </c>
       <c r="E21">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E22">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E23">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" t="s">
         <v>49</v>
       </c>
-      <c r="C24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" t="s">
-        <v>51</v>
-      </c>
       <c r="E24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E25">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
       </c>
       <c r="D26" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E27">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C28" t="s">
         <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E28">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C29" t="s">
         <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E29">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C30" t="s">
         <v>10</v>
       </c>
       <c r="D30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E30">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C31" t="s">
         <v>11</v>
       </c>
       <c r="D31" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E31">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1612,7 +1635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1629,7 +1652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1646,7 +1669,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1663,7 +1686,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1680,7 +1703,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1697,109 +1720,109 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D38" t="s">
         <v>41</v>
       </c>
-      <c r="C38" t="s">
-        <v>42</v>
-      </c>
-      <c r="D38" t="s">
-        <v>43</v>
-      </c>
       <c r="E38">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C39" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D39" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E39">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" t="s">
         <v>41</v>
       </c>
-      <c r="C40" t="s">
-        <v>44</v>
-      </c>
-      <c r="D40" t="s">
-        <v>43</v>
-      </c>
       <c r="E40">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D41" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E41">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C42" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D42" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E42">
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C43" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D43" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E43">
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1809,14 +1832,14 @@
       <c r="C44" t="s">
         <v>13</v>
       </c>
-      <c r="D44" t="s">
-        <v>26</v>
+      <c r="D44" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="E44">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1826,14 +1849,14 @@
       <c r="C45" t="s">
         <v>13</v>
       </c>
-      <c r="D45" t="s">
-        <v>27</v>
+      <c r="D45" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="E45">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1843,14 +1866,14 @@
       <c r="C46" t="s">
         <v>16</v>
       </c>
-      <c r="D46" t="s">
-        <v>26</v>
+      <c r="D46" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="E46">
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1860,14 +1883,14 @@
       <c r="C47" t="s">
         <v>16</v>
       </c>
-      <c r="D47" t="s">
-        <v>27</v>
+      <c r="D47" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="E47">
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1877,14 +1900,14 @@
       <c r="C48" t="s">
         <v>17</v>
       </c>
-      <c r="D48" t="s">
-        <v>26</v>
+      <c r="D48" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="E48">
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1894,14 +1917,14 @@
       <c r="C49" t="s">
         <v>18</v>
       </c>
-      <c r="D49" t="s">
-        <v>27</v>
+      <c r="D49" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="E49">
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1918,7 +1941,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1935,7 +1958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1952,7 +1975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1969,7 +1992,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1986,7 +2009,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2003,106 +2026,140 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C56" t="s">
         <v>13</v>
       </c>
       <c r="D56" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E56">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C57" t="s">
         <v>13</v>
       </c>
       <c r="D57" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E57">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C58" t="s">
         <v>16</v>
       </c>
       <c r="D58" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E58">
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C59" t="s">
         <v>16</v>
       </c>
       <c r="D59" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E59">
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C60" t="s">
         <v>17</v>
       </c>
       <c r="D60" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E60">
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C61" t="s">
         <v>18</v>
       </c>
       <c r="D61" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E61">
         <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>55</v>
+      </c>
+      <c r="C62" t="s">
+        <v>56</v>
+      </c>
+      <c r="D62" t="s">
+        <v>57</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>55</v>
+      </c>
+      <c r="C63" t="s">
+        <v>58</v>
+      </c>
+      <c r="D63" t="s">
+        <v>59</v>
+      </c>
+      <c r="E63">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>